<commit_message>
Fix images for cloud post
</commit_message>
<xml_diff>
--- a/others/Thermal Erosion benchmark.xlsx
+++ b/others/Thermal Erosion benchmark.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Website\others\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\moon519.github.io\others\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -428,8 +428,8 @@
         </c:dLbls>
         <c:gapWidth val="444"/>
         <c:overlap val="-90"/>
-        <c:axId val="477806176"/>
-        <c:axId val="477806568"/>
+        <c:axId val="483337144"/>
+        <c:axId val="483338712"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -492,7 +492,7 @@
         </c:extLst>
       </c:barChart>
       <c:catAx>
-        <c:axId val="477806176"/>
+        <c:axId val="483337144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -605,7 +605,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="477806568"/>
+        <c:crossAx val="483338712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -613,7 +613,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="477806568"/>
+        <c:axId val="483338712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -712,7 +712,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="477806176"/>
+        <c:crossAx val="483337144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1170,11 +1170,11 @@
         </c:dLbls>
         <c:gapWidth val="444"/>
         <c:overlap val="-90"/>
-        <c:axId val="477803432"/>
-        <c:axId val="477804608"/>
+        <c:axId val="483339496"/>
+        <c:axId val="483339888"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="477803432"/>
+        <c:axId val="483339496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1214,14 +1214,14 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="fr-FR" sz="1800"/>
+                  <a:rPr lang="fr-FR" sz="900"/>
                   <a:t>Grid</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="fr-FR" sz="1800" baseline="0"/>
+                  <a:rPr lang="fr-FR" sz="900" baseline="0"/>
                   <a:t> resolution</a:t>
                 </a:r>
-                <a:endParaRPr lang="fr-FR" sz="1800"/>
+                <a:endParaRPr lang="fr-FR" sz="900"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1292,7 +1292,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="477804608"/>
+        <c:crossAx val="483339888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1300,7 +1300,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="477804608"/>
+        <c:axId val="483339888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1399,7 +1399,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="477803432"/>
+        <c:crossAx val="483339496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2934,8 +2934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="J75" sqref="J75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>